<commit_message>
Add placeholder image for socket and update product data in Excel
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -1414,8 +1414,16 @@
       <c r="D36" t="n">
         <v>5</v>
       </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>iVBORw0KGgoAAAANSUhEUgAAAAEAAAABCAQAAAC1HAwCAAAAC0lEQVR4nGNgYAAAAAMAAWgmWQ0AAAAASUVORK5CYII=</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>data/product_images/Socket_placeholder.png</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">

</xml_diff>